<commit_message>
formatted text added code and table screenshots
</commit_message>
<xml_diff>
--- a/Docs/Supporting Docs/Datatypes.xlsx
+++ b/Docs/Supporting Docs/Datatypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\685239\Desktop\dm-assgn\Docs\Supporting Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12C09D9-A15A-4A34-A23A-F6C59C614A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D474F59E-7605-4159-9E9E-8934A63251A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA261F3C-F3E9-4B22-8787-69CD0F8B89A0}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Attrition</t>
   </si>
@@ -157,9 +156,6 @@
     <t>['Sales' 'Research &amp; Development' 'Human Resources']</t>
   </si>
   <si>
-    <t>['2' '1' '4' '3' '5' 'NAN']</t>
-  </si>
-  <si>
     <t>['Life Sciences' 'Other' 'Medical' 'Marketing' 'Technical Degree' 'Human Resources']</t>
   </si>
   <si>
@@ -227,6 +223,18 @@
   </si>
   <si>
     <t>Identifier type</t>
+  </si>
+  <si>
+    <t>QUANTITATIVE ATTRIBUTES (19):</t>
+  </si>
+  <si>
+    <t>QUALITATIVE ATTRIBUTES: (14)</t>
+  </si>
+  <si>
+    <t>['1' '8' '2' '3' '24' '23' '16' '15' '26' '19' '21' '5' '11' '9' '7' '6' '10' '4' '25' '12' '18' '22' '14' '20' '28' '29' '17' '27' '13']</t>
+  </si>
+  <si>
+    <t>['2' '1' '4' '3' '5']</t>
   </si>
 </sst>
 </file>
@@ -250,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +271,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -287,11 +301,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -322,6 +373,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,371 +706,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E129AEC-B761-42EF-AB9A-2B29ABAAA391}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="44.90625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="8.7265625" style="5"/>
+    <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="41.1796875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="D21" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="D27" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="D32" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="D33" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="C36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="8"/>
+      <c r="C37" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added plots for continuous variables
</commit_message>
<xml_diff>
--- a/Docs/Supporting Docs/Datatypes.xlsx
+++ b/Docs/Supporting Docs/Datatypes.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\685239\Desktop\dm-assgn\Docs\Supporting Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D474F59E-7605-4159-9E9E-8934A63251A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C722966-4DCF-47DA-AF6C-9A1A0619C2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA261F3C-F3E9-4B22-8787-69CD0F8B89A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{FA261F3C-F3E9-4B22-8787-69CD0F8B89A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$E$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="67">
   <si>
     <t>Attrition</t>
   </si>
@@ -708,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E129AEC-B761-42EF-AB9A-2B29ABAAA391}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1122,4 +1126,494 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC84A0D-BB92-4D72-8E90-94ACC33081CC}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="2:5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:5" hidden="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <autoFilter ref="B1:E37" xr:uid="{0BC84A0D-BB92-4D72-8E90-94ACC33081CC}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Continuous"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>